<commit_message>
Changes to data files
</commit_message>
<xml_diff>
--- a/Variables_of_importance.xlsx
+++ b/Variables_of_importance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337BF48F-DA2A-4B6B-AFFF-9CBE141E8951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB86DDA-E766-4503-9B6D-7354B53A1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46365" yWindow="5280" windowWidth="21600" windowHeight="11340" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="328">
   <si>
     <t>Code</t>
   </si>
@@ -373,14 +373,658 @@
   </si>
   <si>
     <t>2345 readings</t>
+  </si>
+  <si>
+    <t>DID040</t>
+  </si>
+  <si>
+    <t>How old {was SP/were you} when a doctor or other health professional first told {you/him/her} that {you/he/she} had diabetes or sugar diabetes?</t>
+  </si>
+  <si>
+    <t>DIQ160</t>
+  </si>
+  <si>
+    <t>{Have you/Has SP} ever been told by a doctor or other health professional that {you have/SP has} any of the following: prediabetes, impaired fasting glucose, impaired glucose tolerance, borderline diabetes or that {your/her/his} blood sugar is higher than normal but not high enough to be called diabetes or sugar diabetes?</t>
+  </si>
+  <si>
+    <t>DIQ170</t>
+  </si>
+  <si>
+    <t>{Have you/Has SP} ever been told by a doctor or other health professional that {you have/s/he has} health conditions or a medical or family history that increases {your/his/her} risk for diabetes?</t>
+  </si>
+  <si>
+    <t>DIQ172</t>
+  </si>
+  <si>
+    <t>{Do you/Does SP} feel {you/he/she} could be at risk for diabetes or prediabetes?</t>
+  </si>
+  <si>
+    <t>DIQ175A</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175A - Family history</t>
+  </si>
+  <si>
+    <t>DIQ175B</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175B - Overweight</t>
+  </si>
+  <si>
+    <t>DIQ175C</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175C - Age</t>
+  </si>
+  <si>
+    <t>DIQ175D</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175D - Poor diet</t>
+  </si>
+  <si>
+    <t>DIQ175E</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175E - Race</t>
+  </si>
+  <si>
+    <t>DIQ175F</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175F - Had a baby weighed over 9 lbs. at birth</t>
+  </si>
+  <si>
+    <t>DIQ175G</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175G - Lack of physical activity</t>
+  </si>
+  <si>
+    <t>DIQ175H</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175H - High blood pressure</t>
+  </si>
+  <si>
+    <t>DIQ175I</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175I - High blood sugar</t>
+  </si>
+  <si>
+    <t>DIQ175J</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175J - High cholesterol</t>
+  </si>
+  <si>
+    <t>DIQ175K</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175K - Hypoglycemic</t>
+  </si>
+  <si>
+    <t>DIQ175L</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175L - Extreme hunger</t>
+  </si>
+  <si>
+    <t>DIQ175M</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175M - Tingling/numbness in hands or feet</t>
+  </si>
+  <si>
+    <t>DIQ175N</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175N - Blurred vision</t>
+  </si>
+  <si>
+    <t>DIQ175O</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175O - Increased fatigue</t>
+  </si>
+  <si>
+    <t>DIQ175P</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175P - Anyone could be at risk</t>
+  </si>
+  <si>
+    <t>DIQ175Q</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175Q - Doctor warning</t>
+  </si>
+  <si>
+    <t>DIQ175R</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175R - Other, specify</t>
+  </si>
+  <si>
+    <t>DIQ175S</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175S - Gestational diabetes</t>
+  </si>
+  <si>
+    <t>DIQ175T</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175T - Frequent urination</t>
+  </si>
+  <si>
+    <t>DIQ175U</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?] DIQ175U - Thirst</t>
+  </si>
+  <si>
+    <t>DIQ175V</t>
+  </si>
+  <si>
+    <t>Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? DIQ175V - Craving for sweet/eating a lot of sugar</t>
+  </si>
+  <si>
+    <t>DIQ180</t>
+  </si>
+  <si>
+    <t>{Have you/Has SP} had a blood test for high blood sugar or diabetes within the past three years?</t>
+  </si>
+  <si>
+    <t>DIQ050</t>
+  </si>
+  <si>
+    <t>{Is SP/Are you} now taking insulin</t>
+  </si>
+  <si>
+    <t>DID060</t>
+  </si>
+  <si>
+    <t>For how long {have you/has SP} been taking insulin?</t>
+  </si>
+  <si>
+    <t>DIQ060U</t>
+  </si>
+  <si>
+    <t>UNIT OF MEASURE (Months/Years UOM for question DID060)</t>
+  </si>
+  <si>
+    <t>DIQ070</t>
+  </si>
+  <si>
+    <t>{Is SP/Are you} now taking diabetic pills to lower {{his/her}/your} blood sugar? These are sometimes called oral agents or oral hypoglycemic agents.</t>
+  </si>
+  <si>
+    <t>DIQ230</t>
+  </si>
+  <si>
+    <t>When was the last time {you/SP} saw a diabetes nurse educator or dietitian or nutritionist for {your/his/her} diabetes? Do not include doctors or other health professionals.</t>
+  </si>
+  <si>
+    <t>DIQ240</t>
+  </si>
+  <si>
+    <t>Is there one doctor or other health professional {you usually see/SP usually sees} for {your/his/her} diabetes? Do not include specialists to whom {you have/SP has} been referred such as diabetes educators, dieticians or foot and eye doctors.</t>
+  </si>
+  <si>
+    <t>DID250</t>
+  </si>
+  <si>
+    <t>How many times {have you/has SP} seen this doctor or other health professional in the past 12 months?</t>
+  </si>
+  <si>
+    <t>DID260</t>
+  </si>
+  <si>
+    <t>How often {do you check your/does SP check his/her} blood for glucose or sugar? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</t>
+  </si>
+  <si>
+    <t>DIQ260U</t>
+  </si>
+  <si>
+    <t>DIQ275</t>
+  </si>
+  <si>
+    <t>Glycosylated (GLY-KOH-SIH-LAY-TED) hemoglobin or the "A one C" test measures your average level of blood sugar for the past 3 months, and usually ranges between 5.0 and 13.9. During the past 12 months, has a doctor or other health professional checked {your/SP's} glycosylated hemoglobin or "A one C"?</t>
+  </si>
+  <si>
+    <t>DBD895</t>
+  </si>
+  <si>
+    <t>Next I'm going to ask you about meals. By meal, I mean breakfast, lunch and dinner. During the past 7 days, how many meals {did you/did SP} get that were prepared away from home in places such as restaurants, fast food places, food stands, grocery stores, or from vending machines? {Please do not include meals provided as part of the school lunch or school breakfast./Please do not include meals provided as part of the community programs you reported earlier.}</t>
+  </si>
+  <si>
+    <t>DBD900</t>
+  </si>
+  <si>
+    <t>How many of those meals {did you/did SP} get from a fast-food or pizza place?</t>
+  </si>
+  <si>
+    <t>DBD905</t>
+  </si>
+  <si>
+    <t>Some grocery stores sell "ready to eat" foods such as salads, soups, chicken, sandwiches and cooked vegetables in their salad bars and deli counters. During the past 30 days, how often did {you/SP} eat "ready to eat" foods from the grocery store? Please do not include sliced meat or cheese you buy for sandwiches and frozen or canned foods.</t>
+  </si>
+  <si>
+    <t>DBD910</t>
+  </si>
+  <si>
+    <t>During the past 30 days, how often did you {SP} eat frozen meals or frozen pizzas? Here are some examples of frozen meals and frozen pizzas.</t>
+  </si>
+  <si>
+    <t>CBQ596</t>
+  </si>
+  <si>
+    <t>Next I'm going to ask a few questions about the nutritional guidelines recommended for Americans by the federal government. {Have you/Has SP} heard of My Plate?</t>
+  </si>
+  <si>
+    <t>CBQ606</t>
+  </si>
+  <si>
+    <t>{Have you/Has SP} looked up the My Plate plan on the internet?</t>
+  </si>
+  <si>
+    <t>CBQ611</t>
+  </si>
+  <si>
+    <t>{Have you/Has SP} tried to follow the recommendations in the My Plate plan?</t>
+  </si>
+  <si>
+    <t>DIQ010</t>
+  </si>
+  <si>
+    <t>The next questions are about specific medical conditions. {Other than during pregnancy, {have you/has SP}/{Have you/Has SP}} ever been told by a doctor or health professional that {you have/{he/she/SP} has} diabetes or sugar diabetes?</t>
+  </si>
+  <si>
+    <t>Indicates # of times food consumed outside</t>
+  </si>
+  <si>
+    <t>Indicates # of times food consumed from unhealthy sources</t>
+  </si>
+  <si>
+    <t>Indicates # of times food consumed falls within healthy category</t>
+  </si>
+  <si>
+    <t>Indicates # of times processed frozen food is consumed</t>
+  </si>
+  <si>
+    <t>Indicates nutritional knowledge/awareness</t>
+  </si>
+  <si>
+    <t>CBQ505</t>
+  </si>
+  <si>
+    <t>{I'll tell you when you will need it.} For the first few questions, please answer yes or no. In the past 12 months, did you buy food from fast food or pizza places? SP interview version: In the past 12 months, did {you/SP} buy food from fast food or pizza places?</t>
+  </si>
+  <si>
+    <t>CBQ535</t>
+  </si>
+  <si>
+    <t>The last time when you ate out or bought food at a fast-food or pizza place, did you see nutrition or health information about any foods on the menu? SP interview version: The last time when {you/SP} ate out or bought food at a fast-food or pizza place, did {you/he/she} see nutrition or health information about any foods on the menu?</t>
+  </si>
+  <si>
+    <t>CBQ540</t>
+  </si>
+  <si>
+    <t>Did you use the information in deciding which foods to buy? SP interview version: Did {you/SP} use the information in deciding which foods to buy?</t>
+  </si>
+  <si>
+    <t>CBQ545</t>
+  </si>
+  <si>
+    <t>{Please open your hand card booklet and turn to hand card 1 to answer the next question.} If nutrition or health information were readily available in fast food or pizza places, would you use it often, sometimes, rarely, or never, in deciding what to order? SP interview version: If nutrition or health information were readily available in fast food or pizza places, would {you/SP} use it often, sometimes, rarely, or never, in deciding what to order?</t>
+  </si>
+  <si>
+    <t>FSD151</t>
+  </si>
+  <si>
+    <t>In the last 12 months, did {you/you or any member of your household} ever get emergency food from a church, a food pantry, or a food bank, or eat in a soup kitchen?</t>
+  </si>
+  <si>
+    <t>FSQ165</t>
+  </si>
+  <si>
+    <t>The next questions are about SNAP, the Supplemental Nutrition Assistance Program, formerly known as the Food Stamp Program. SNAP benefits are provided on an electronic debit card {or EBT card} {called the DISPLAY STATE NAME FOR EBT CARD}} card in STATE}. Have {you/you or anyone in your household} ever received SNAP or Food Stamp benefits?</t>
+  </si>
+  <si>
+    <t>FSQ012</t>
+  </si>
+  <si>
+    <t>In the last 12 months, did {you/you or any member of your household} receive SNAP or Food Stamp benefits?</t>
+  </si>
+  <si>
+    <t>FSD012N</t>
+  </si>
+  <si>
+    <t>In the last 12 months, how many people in your household received SNAP or Food Stamp benefits?</t>
+  </si>
+  <si>
+    <t>FSD230</t>
+  </si>
+  <si>
+    <t>{Do you/Does any member of your household} currently receive SNAP or Food Stamp benefits?</t>
+  </si>
+  <si>
+    <t>FSD225</t>
+  </si>
+  <si>
+    <t>Number of days between the time the household last received Food Stamp benefit and the date of interview.</t>
+  </si>
+  <si>
+    <t>FSQ235</t>
+  </si>
+  <si>
+    <t>How much did {you/your household} receive in food stamp benefits the last time you got them? ENTER DOLLAR AMOUNT.</t>
+  </si>
+  <si>
+    <t>Indicative of SES status</t>
+  </si>
+  <si>
+    <t>DBQ700</t>
+  </si>
+  <si>
+    <t>Next I have some questions about {your/SP?s} eating habits. In general, how healthy is {your/his/her} overall diet? Would you say . . .</t>
+  </si>
+  <si>
+    <t>Self-perceived dietary quality</t>
+  </si>
+  <si>
+    <t>DPQ010</t>
+  </si>
+  <si>
+    <t>Over the last 2 weeks, how often have you been bothered by the following problems: little interest or pleasure in doing things? Would you say...</t>
+  </si>
+  <si>
+    <t>DPQ020</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] feeling down, depressed, or hopeless?</t>
+  </si>
+  <si>
+    <t>DPQ030</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] trouble falling or staying asleep, or sleeping too much?</t>
+  </si>
+  <si>
+    <t>DPQ040</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] feeling tired or having little energy?</t>
+  </si>
+  <si>
+    <t>DPQ050</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] poor appetite or overeating?</t>
+  </si>
+  <si>
+    <t>DPQ060</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] feeling bad about yourself - or that you are a failure or have let yourself or your family down?</t>
+  </si>
+  <si>
+    <t>DPQ070</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] trouble concentrating on things, such as reading the newspaper or watching TV?</t>
+  </si>
+  <si>
+    <t>DPQ080</t>
+  </si>
+  <si>
+    <t>[Over the last 2 weeks, how often have you been bothered by the following problems:] moving or speaking so slowly that other people could have noticed? Or the opposite - being so fidgety or restless that you have been moving around a lot more than usual?</t>
+  </si>
+  <si>
+    <t>DPQ090</t>
+  </si>
+  <si>
+    <t>Over the last 2 weeks, how often have you been bothered by the following problems: Thoughts that you would be better off dead or of hurting yourself in some way?</t>
+  </si>
+  <si>
+    <t>DPQ100</t>
+  </si>
+  <si>
+    <t>How difficult have these problems made it for you to do your work, take care of things at home, or get along with people?</t>
+  </si>
+  <si>
+    <t>Mental health - Tabulate into mental health score and correlate with diabetes</t>
+  </si>
+  <si>
+    <t>Consider removing as this not useful for diagnosing new diabetics?</t>
+  </si>
+  <si>
+    <t>737 respondents - Target variable for diabetes/non-diabetes?</t>
+  </si>
+  <si>
+    <t>Increased risk as identified by health professional</t>
+  </si>
+  <si>
+    <t>Self-perceived diabetes risk</t>
+  </si>
+  <si>
+    <t>PAQ605</t>
+  </si>
+  <si>
+    <t>Next I am going to ask you about the time {you spend/SP spends} doing different types of physical activity in a typical week. Think first about the time {you spend/he spends/she spends} doing work. Think of work as the things that {you have/he has/she has} to do such as paid or unpaid work, household chores, and yard work. Does {your/SP's} work involve vigorous-intensity activity that causes large increases in breathing or heart rate like carrying or lifting heavy loads, digging or construction work for at least 10 minutes continuously?</t>
+  </si>
+  <si>
+    <t>PAQ610</t>
+  </si>
+  <si>
+    <t>In a typical week, on how many days {do you/does SP} do vigorous-intensity activities as part of {your/his/her} work?</t>
+  </si>
+  <si>
+    <t>PAD615</t>
+  </si>
+  <si>
+    <t>How much time {do you/does SP} spend doing vigorous-intensity activities at work on a typical day?</t>
+  </si>
+  <si>
+    <t>PAQ620</t>
+  </si>
+  <si>
+    <t>Does {your/SP's} work involve moderate-intensity activity that causes small increases in breathing or heart rate such as brisk walking or carrying light loads for at least 10 minutes continuously?</t>
+  </si>
+  <si>
+    <t>PAQ625</t>
+  </si>
+  <si>
+    <t>In a typical week, on how many days {do you/does SP} do moderate-intensity activities as part of {your/his/her} work?</t>
+  </si>
+  <si>
+    <t>PAD630</t>
+  </si>
+  <si>
+    <t>How much time {do you/does SP} spend doing moderate-intensity activities at work on a typical day?</t>
+  </si>
+  <si>
+    <t>PAQ635</t>
+  </si>
+  <si>
+    <t>The next questions exclude the physical activity at work that you have already mentioned. Now I would like to ask you about the usual way {you travel/SP travels} to and from places. For example to school, for shopping, to work. In a typical week {do you/does SP} walk or use a bicycle for at least 10 minutes continuously to get to and from places?</t>
+  </si>
+  <si>
+    <t>PAQ640</t>
+  </si>
+  <si>
+    <t>In a typical week, on how many days {do you/does SP} walk or bicycle for at least 10 minutes continuously to get to and from places?</t>
+  </si>
+  <si>
+    <t>PAD645</t>
+  </si>
+  <si>
+    <t>How much time {do you/does SP} spend walking or bicycling for travel on a typical day?</t>
+  </si>
+  <si>
+    <t>PAQ650</t>
+  </si>
+  <si>
+    <t>The next questions exclude the work and transport activities that you have already mentioned. Now I would like to ask you about sports, fitness and recreational activities. In a typical week {do you/does SP} do any vigorous-intensity sports, fitness, or recreational activities that cause large increases in breathing or heart rate like running or basketball for at least 10 minutes continuously?</t>
+  </si>
+  <si>
+    <t>PAQ655</t>
+  </si>
+  <si>
+    <t>In a typical week, on how many days {do you/does SP} do vigorous-intensity sports, fitness or recreational activities?</t>
+  </si>
+  <si>
+    <t>PAD660</t>
+  </si>
+  <si>
+    <t>How much time {do you/does SP} spend doing vigorous-intensity sports, fitness or recreational activities on a typical day?</t>
+  </si>
+  <si>
+    <t>PAQ665</t>
+  </si>
+  <si>
+    <t>In a typical week {do you/does SP} do any moderate-intensity sports, fitness, or recreational activities that cause a small increase in breathing or heart rate such as brisk walking, bicycling, swimming, or volleyball for at least 10 minutes continuously?</t>
+  </si>
+  <si>
+    <t>PAQ670</t>
+  </si>
+  <si>
+    <t>In a typical week, on how many days {do you/does SP} do moderate-intensity sports, fitness or recreational activities?</t>
+  </si>
+  <si>
+    <t>PAD675</t>
+  </si>
+  <si>
+    <t>How much time {do you/does SP} spend doing moderate-intensity sports, fitness or recreational activities on a typical day?</t>
+  </si>
+  <si>
+    <t>PAD680</t>
+  </si>
+  <si>
+    <t>The following question is about sitting at school, at home, getting to and from places, or with friends including time spent sitting at a desk, traveling in a car or bus, reading, playing cards, watching television, or using a computer. Do not include time spent sleeping. How much time {do you/does SP} usually spend sitting on a typical day?</t>
+  </si>
+  <si>
+    <t>PAQ706</t>
+  </si>
+  <si>
+    <t>I'd like to ask you some questions about {your/SP's} activities. During the past 7 days, on how many days {were you/was SP} physically active for a total of at least 60 minutes per day? Add up all the time {you/he/she} spent in any kind of physical activity that increased {your/his/her} heart rate and made {you/him/her} breathe hard some of the time.</t>
+  </si>
+  <si>
+    <t>PAQ710</t>
+  </si>
+  <si>
+    <t>Now I will ask you first about TV watching and then about computer use. Over the past 30 days, on average how many hours per day did {you/SP} sit and watch TV or videos? Would you say . . .</t>
+  </si>
+  <si>
+    <t>PAQ715</t>
+  </si>
+  <si>
+    <t>Over the past 30 days, on average how many hours per day did {you/SP} use a computer or play computer games outside of school? Include Playstation, Nintendo DS, or other portable video games Would you say . . .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHQ070 </t>
+  </si>
+  <si>
+    <t>Tried to lose weight in past year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHQ030 </t>
+  </si>
+  <si>
+    <t>How do you consider your weight</t>
+  </si>
+  <si>
+    <t>Self perception of weight and health</t>
+  </si>
+  <si>
+    <t>Identifying intent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBDHDDSI </t>
+  </si>
+  <si>
+    <t>Direct HDL-Cholesterol (mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBDTRSI </t>
+  </si>
+  <si>
+    <t>Triglyceride (mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBDLDLSI </t>
+  </si>
+  <si>
+    <t>LDL-cholesterol (mmol/L)</t>
+  </si>
+  <si>
+    <t>3105 readings</t>
+  </si>
+  <si>
+    <t>3146 readings</t>
+  </si>
+  <si>
+    <t>7624 readings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBDTCSI </t>
+  </si>
+  <si>
+    <t>Total Cholesterol( mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBXIN </t>
+  </si>
+  <si>
+    <t>Insulin (uU/mL)</t>
+  </si>
+  <si>
+    <t>3093 readings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHAFSTMN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total length of 'food fast', minutes </t>
+  </si>
+  <si>
+    <t>To attenuate fasting glucose levels (LBDGLUSI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBXVIDMS </t>
+  </si>
+  <si>
+    <t>8437 readings</t>
+  </si>
+  <si>
+    <t>Vitamin D levels 25OHD2+25OHD3 (nmol/L)</t>
+  </si>
+  <si>
+    <t>Total length of 'food fast', minutes</t>
+  </si>
+  <si>
+    <t>To attenuate fasting insulin levels (LBXIN)</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -408,8 +1052,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,27 +1372,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="115.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.5703125" customWidth="1"/>
     <col min="4" max="4" width="83.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -848,72 +1500,60 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,10 +1561,10 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,10 +1572,10 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -943,10 +1583,10 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,68 +1594,68 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,13 +1663,10 @@
         <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,10 +1674,10 @@
         <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,10 +1685,10 @@
         <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,10 +1696,10 @@
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,10 +1707,10 @@
         <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,10 +1718,13 @@
         <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,10 +1732,13 @@
         <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,10 +1746,13 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,10 +1760,13 @@
         <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,10 +1774,13 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,13 +1788,13 @@
         <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,13 +1802,10 @@
         <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,13 +1813,13 @@
         <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,13 +1827,13 @@
         <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,80 +1841,83 @@
         <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>319</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>320</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>306</v>
       </c>
       <c r="D41" t="s">
-        <v>104</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>307</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>308</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,13 +1925,13 @@
         <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>310</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,18 +1939,1213 @@
         <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>314</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>315</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s">
+        <v>316</v>
+      </c>
+      <c r="C45" t="s">
+        <v>317</v>
+      </c>
+      <c r="D45" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" t="s">
+        <v>319</v>
+      </c>
+      <c r="C46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D46" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
+        <v>322</v>
+      </c>
+      <c r="C47" t="s">
+        <v>324</v>
+      </c>
+      <c r="D47" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>233</v>
+      </c>
+      <c r="C48" t="s">
+        <v>234</v>
+      </c>
+      <c r="D48" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>117</v>
+      </c>
+      <c r="D50" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B79" t="s">
+        <v>174</v>
+      </c>
+      <c r="C79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" t="s">
+        <v>176</v>
+      </c>
+      <c r="C80" t="s">
+        <v>177</v>
+      </c>
+      <c r="D80" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81" t="s">
+        <v>179</v>
+      </c>
+      <c r="D81" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" t="s">
+        <v>180</v>
+      </c>
+      <c r="C82" t="s">
+        <v>181</v>
+      </c>
+      <c r="D82" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" t="s">
+        <v>185</v>
+      </c>
+      <c r="D84" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>33</v>
+      </c>
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="s">
+        <v>185</v>
+      </c>
+      <c r="D85" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" t="s">
+        <v>188</v>
+      </c>
+      <c r="D86" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>189</v>
+      </c>
+      <c r="C87" t="s">
+        <v>190</v>
+      </c>
+      <c r="D87" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>33</v>
+      </c>
+      <c r="B88" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" t="s">
+        <v>192</v>
+      </c>
+      <c r="D88" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>33</v>
+      </c>
+      <c r="B89" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" t="s">
+        <v>194</v>
+      </c>
+      <c r="D89" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>33</v>
+      </c>
+      <c r="B90" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" t="s">
+        <v>196</v>
+      </c>
+      <c r="D90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" t="s">
+        <v>199</v>
+      </c>
+      <c r="C92" t="s">
+        <v>200</v>
+      </c>
+      <c r="D92" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>33</v>
+      </c>
+      <c r="B93" t="s">
+        <v>201</v>
+      </c>
+      <c r="C93" t="s">
+        <v>202</v>
+      </c>
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>33</v>
+      </c>
+      <c r="B94" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" t="s">
+        <v>211</v>
+      </c>
+      <c r="D94" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>33</v>
+      </c>
+      <c r="B95" t="s">
+        <v>212</v>
+      </c>
+      <c r="C95" t="s">
+        <v>213</v>
+      </c>
+      <c r="D95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B96" t="s">
+        <v>214</v>
+      </c>
+      <c r="C96" t="s">
+        <v>215</v>
+      </c>
+      <c r="D96" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" t="s">
+        <v>217</v>
+      </c>
+      <c r="D97" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>33</v>
+      </c>
+      <c r="B98" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" t="s">
+        <v>219</v>
+      </c>
+      <c r="D98" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>33</v>
+      </c>
+      <c r="B101" t="s">
+        <v>224</v>
+      </c>
+      <c r="C101" t="s">
+        <v>225</v>
+      </c>
+      <c r="D101" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>33</v>
+      </c>
+      <c r="B102" t="s">
+        <v>226</v>
+      </c>
+      <c r="C102" t="s">
+        <v>227</v>
+      </c>
+      <c r="D102" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>33</v>
+      </c>
+      <c r="B103" t="s">
+        <v>228</v>
+      </c>
+      <c r="C103" t="s">
+        <v>229</v>
+      </c>
+      <c r="D103" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>33</v>
+      </c>
+      <c r="B104" t="s">
+        <v>230</v>
+      </c>
+      <c r="C104" t="s">
+        <v>231</v>
+      </c>
+      <c r="D104" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>33</v>
+      </c>
+      <c r="B105" t="s">
+        <v>236</v>
+      </c>
+      <c r="C105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D105" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106" t="s">
+        <v>238</v>
+      </c>
+      <c r="C106" t="s">
+        <v>239</v>
+      </c>
+      <c r="D106" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>33</v>
+      </c>
+      <c r="B107" t="s">
+        <v>240</v>
+      </c>
+      <c r="C107" t="s">
+        <v>241</v>
+      </c>
+      <c r="D107" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>33</v>
+      </c>
+      <c r="B108" t="s">
+        <v>242</v>
+      </c>
+      <c r="C108" t="s">
+        <v>243</v>
+      </c>
+      <c r="D108" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>33</v>
+      </c>
+      <c r="B109" t="s">
+        <v>244</v>
+      </c>
+      <c r="C109" t="s">
+        <v>245</v>
+      </c>
+      <c r="D109" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B110" t="s">
+        <v>246</v>
+      </c>
+      <c r="C110" t="s">
+        <v>247</v>
+      </c>
+      <c r="D110" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>33</v>
+      </c>
+      <c r="B111" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" t="s">
+        <v>249</v>
+      </c>
+      <c r="D111" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>33</v>
+      </c>
+      <c r="B112" t="s">
+        <v>250</v>
+      </c>
+      <c r="C112" t="s">
+        <v>251</v>
+      </c>
+      <c r="D112" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" t="s">
+        <v>252</v>
+      </c>
+      <c r="C113" t="s">
+        <v>253</v>
+      </c>
+      <c r="D113" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>33</v>
+      </c>
+      <c r="B114" t="s">
+        <v>254</v>
+      </c>
+      <c r="C114" t="s">
+        <v>255</v>
+      </c>
+      <c r="D114" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>33</v>
+      </c>
+      <c r="B115" t="s">
+        <v>261</v>
+      </c>
+      <c r="C115" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" t="s">
+        <v>263</v>
+      </c>
+      <c r="C116" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>33</v>
+      </c>
+      <c r="B117" t="s">
+        <v>265</v>
+      </c>
+      <c r="C117" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>33</v>
+      </c>
+      <c r="B118" t="s">
+        <v>267</v>
+      </c>
+      <c r="C118" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>33</v>
+      </c>
+      <c r="B119" t="s">
+        <v>269</v>
+      </c>
+      <c r="C119" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>33</v>
+      </c>
+      <c r="B120" t="s">
+        <v>271</v>
+      </c>
+      <c r="C120" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>33</v>
+      </c>
+      <c r="B121" t="s">
+        <v>273</v>
+      </c>
+      <c r="C121" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>33</v>
+      </c>
+      <c r="B122" t="s">
+        <v>275</v>
+      </c>
+      <c r="C122" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>33</v>
+      </c>
+      <c r="B123" t="s">
+        <v>277</v>
+      </c>
+      <c r="C123" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>33</v>
+      </c>
+      <c r="B124" t="s">
+        <v>279</v>
+      </c>
+      <c r="C124" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>33</v>
+      </c>
+      <c r="B125" t="s">
+        <v>281</v>
+      </c>
+      <c r="C125" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>33</v>
+      </c>
+      <c r="B126" t="s">
+        <v>283</v>
+      </c>
+      <c r="C126" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>33</v>
+      </c>
+      <c r="B127" t="s">
+        <v>285</v>
+      </c>
+      <c r="C127" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>33</v>
+      </c>
+      <c r="B128" t="s">
+        <v>287</v>
+      </c>
+      <c r="C128" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>33</v>
+      </c>
+      <c r="B129" t="s">
+        <v>289</v>
+      </c>
+      <c r="C129" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130" t="s">
+        <v>291</v>
+      </c>
+      <c r="C130" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>33</v>
+      </c>
+      <c r="B131" t="s">
+        <v>293</v>
+      </c>
+      <c r="C131" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>33</v>
+      </c>
+      <c r="B132" t="s">
+        <v>295</v>
+      </c>
+      <c r="C132" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>33</v>
+      </c>
+      <c r="B133" t="s">
+        <v>297</v>
+      </c>
+      <c r="C133" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>33</v>
+      </c>
+      <c r="B134" t="s">
+        <v>301</v>
+      </c>
+      <c r="C134" t="s">
+        <v>302</v>
+      </c>
+      <c r="D134" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>33</v>
+      </c>
+      <c r="B135" t="s">
+        <v>299</v>
+      </c>
+      <c r="C135" t="s">
+        <v>300</v>
+      </c>
+      <c r="D135" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>33</v>
+      </c>
+      <c r="B136" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>26</v>
+      </c>
+      <c r="D136" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>33</v>
+      </c>
+      <c r="B137" t="s">
+        <v>27</v>
+      </c>
+      <c r="C137" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>33</v>
+      </c>
+      <c r="B138" t="s">
+        <v>29</v>
+      </c>
+      <c r="C138" t="s">
+        <v>30</v>
+      </c>
+      <c r="D138" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>33</v>
+      </c>
+      <c r="B139" t="s">
+        <v>34</v>
+      </c>
+      <c r="C139" t="s">
+        <v>35</v>
+      </c>
+      <c r="D139" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>33</v>
+      </c>
+      <c r="B140" t="s">
+        <v>36</v>
+      </c>
+      <c r="C140" t="s">
+        <v>37</v>
+      </c>
+      <c r="D140" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Categorised Physical Activity Indicators
</commit_message>
<xml_diff>
--- a/Variables_of_importance.xlsx
+++ b/Variables_of_importance.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED805D4-582B-4A09-9721-D84E23F47790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53BE16E-80ED-4706-A4C9-D8BDA090F6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Physical Activity Indicator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="215">
   <si>
     <t>Code</t>
   </si>
@@ -631,6 +632,45 @@
   </si>
   <si>
     <t>Weight change summary stat</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Vigorous Intensity</t>
+  </si>
+  <si>
+    <t>Moderate Intensity</t>
+  </si>
+  <si>
+    <t>Light Intensity</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
+    <t>Sitting</t>
+  </si>
+  <si>
+    <t>Activity &gt;60min</t>
+  </si>
+  <si>
+    <t>TV Use</t>
+  </si>
+  <si>
+    <t>Computer Use</t>
   </si>
 </sst>
 </file>
@@ -686,11 +726,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,19 +1048,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="142.7109375" customWidth="1"/>
-    <col min="4" max="4" width="92.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.7265625" customWidth="1"/>
+    <col min="4" max="4" width="92.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1061,7 +1102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1103,7 +1144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1155,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1128,7 +1169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1139,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1191,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1161,7 +1202,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1172,7 +1213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1233,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1201,7 +1242,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1212,7 +1253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1226,7 +1267,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1240,7 +1281,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1254,7 +1295,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1268,7 +1309,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1282,7 +1323,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1296,7 +1337,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1310,7 +1351,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1324,7 +1365,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1338,7 +1379,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1352,7 +1393,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1366,7 +1407,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1380,7 +1421,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1391,7 +1432,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1405,7 +1446,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1419,7 +1460,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1433,7 +1474,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1447,7 +1488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1461,7 +1502,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1475,7 +1516,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1530,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1503,7 +1544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1517,7 +1558,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1531,7 +1572,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1545,7 +1586,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1559,7 +1600,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -1573,7 +1614,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1587,13 +1628,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1607,7 +1648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1621,7 +1662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1635,7 +1676,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -1649,7 +1690,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -1663,7 +1704,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -1677,7 +1718,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -1691,7 +1732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -1705,7 +1746,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -1719,7 +1760,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -1733,7 +1774,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -1747,7 +1788,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -1761,13 +1802,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -1778,7 +1819,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -1789,7 +1830,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -1800,7 +1841,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -1811,7 +1852,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -1822,7 +1863,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -1833,7 +1874,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -1844,7 +1885,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -1855,7 +1896,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -1866,7 +1907,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>31</v>
       </c>
@@ -1877,7 +1918,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1929,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -1899,7 +1940,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -1910,7 +1951,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>31</v>
       </c>
@@ -1921,7 +1962,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -1932,7 +1973,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -1943,7 +1984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>31</v>
       </c>
@@ -1954,7 +1995,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -1965,7 +2006,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -1976,13 +2017,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -1996,7 +2037,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>31</v>
       </c>
@@ -2010,7 +2051,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -2024,13 +2065,13 @@
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>31</v>
       </c>
@@ -2044,7 +2085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -2058,7 +2099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>34</v>
       </c>
@@ -2069,7 +2110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B85" s="3"/>
       <c r="C85" s="3" t="s">
         <v>201</v>
@@ -2079,4 +2120,428 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB70F0A3-C5F6-4675-89FB-258EF444123F}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="85.36328125" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data cleaning and importing Bryan's file
</commit_message>
<xml_diff>
--- a/Variables_of_importance.xlsx
+++ b/Variables_of_importance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949AECDA-7EAD-4144-A8D1-97D12CE7460B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B71D34-E52C-40DB-BF09-ED77E5478BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="181">
   <si>
     <t>Code</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Mental health - Tabulate into mental health score and correlate with diabetes</t>
   </si>
   <si>
-    <t>Increased risk as identified by health professional</t>
-  </si>
-  <si>
     <t>PAQ605</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>6464 readings Self-perceived dietary quality</t>
   </si>
   <si>
-    <t>6469 readings Self-perceived diabetes risk</t>
-  </si>
-  <si>
     <t>Mental Health Questionnaire</t>
   </si>
   <si>
@@ -540,9 +534,6 @@
     <t>6568 readings</t>
   </si>
   <si>
-    <t>1338 readings - One hot encoding</t>
-  </si>
-  <si>
     <t>Indicative of SES status ~6000 entries</t>
   </si>
   <si>
@@ -565,6 +556,57 @@
   </si>
   <si>
     <t>General health condition</t>
+  </si>
+  <si>
+    <r>
+      <t>6469 readings Self-perceived diabetes risk</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Not applicable - Question was asked to people without diabetes)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1338 readings - One hot encoding</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Not applicable - Question was asked to people without diabetes)</t>
+    </r>
+  </si>
+  <si>
+    <t>(Not applicable - Question was only asked to people without diabetes)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increased risk as identified by health professional </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Not applicable - Question was only asked to people without diabetes)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -588,7 +630,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +655,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -626,12 +674,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1055,7 +1104,7 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,10 +1182,10 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,10 +1194,10 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,13 +1216,13 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,7 +1236,7 @@
         <v>55</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1201,7 +1250,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,13 +1258,13 @@
         <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" t="s">
         <v>150</v>
-      </c>
-      <c r="D20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,13 +1272,13 @@
         <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,13 +1286,13 @@
         <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" t="s">
         <v>154</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,66 +1300,69 @@
         <v>56</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
         <v>159</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D23" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>60</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,7 +1432,7 @@
         <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,13 +1446,13 @@
         <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,7 +1626,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,10 +1634,10 @@
         <v>31</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1593,10 +1645,10 @@
         <v>31</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,10 +1656,10 @@
         <v>31</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,10 +1667,10 @@
         <v>31</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1626,10 +1678,10 @@
         <v>31</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1637,10 +1689,10 @@
         <v>31</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1648,10 +1700,10 @@
         <v>31</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1659,10 +1711,10 @@
         <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1670,10 +1722,10 @@
         <v>31</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,10 +1733,10 @@
         <v>31</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1692,10 +1744,10 @@
         <v>31</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1703,10 +1755,10 @@
         <v>31</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1714,10 +1766,10 @@
         <v>31</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1725,10 +1777,10 @@
         <v>31</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1736,10 +1788,10 @@
         <v>31</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1747,10 +1799,10 @@
         <v>31</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1758,10 +1810,10 @@
         <v>31</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,16 +1821,16 @@
         <v>31</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,13 +1838,13 @@
         <v>31</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" t="s">
         <v>146</v>
-      </c>
-      <c r="D67" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1800,13 +1852,13 @@
         <v>31</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="D68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,7 +1872,7 @@
         <v>84</v>
       </c>
       <c r="D69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,16 +1880,16 @@
         <v>31</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,7 +1934,7 @@
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to main file
</commit_message>
<xml_diff>
--- a/Variables_of_importance.xlsx
+++ b/Variables_of_importance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B71D34-E52C-40DB-BF09-ED77E5478BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2208F7F7-397E-44F3-AEE9-65A2A647F8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
@@ -998,7 +998,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,10 +1027,10 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -1041,10 +1041,10 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -1932,8 +1932,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-      <c r="C75" s="3" t="s">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>